<commit_message>
Issue - #9:Done, #17:Done, #18 추가
</commit_message>
<xml_diff>
--- a/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
+++ b/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="Issue list" sheetId="1" r:id="rId1"/>
     <sheet name="ECO list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" calcMode="manual"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -258,10 +258,6 @@
   </si>
   <si>
     <t>SW</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OPEN</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -479,6 +475,25 @@
   <si>
     <t>Plasma_Gen_Main Board_SCH_V2.0_20180102.sch
 Plasma_Gen_Main Board_PCB_V1.0_20180102.pcb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능 구현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low Battery시 LED_R Blink 동작하지 않음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Chargetask_lowbatt.c / Chargetask_state.h 수정 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RS-232 동작 안됨
+ - RX interrupt 인식을 못함
+ - USART1_RX date의 Low level이 2.17V 까지밖에 안떨어짐(정상 0V)
+ - MAX3232의 ChargePump의 파형이 점검치구 board와 틀림</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1126,7 +1141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1161,7 +1176,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1372,9 +1387,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1443,7 +1458,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I4" s="48"/>
     </row>
@@ -1467,10 +1482,10 @@
         <v>11</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
@@ -1588,10 +1603,10 @@
         <v>43099</v>
       </c>
       <c r="G10" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="32" t="s">
         <v>61</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>62</v>
       </c>
       <c r="I10" s="34"/>
     </row>
@@ -1612,32 +1627,36 @@
         <v>43099</v>
       </c>
       <c r="G11" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="34"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="29">
+        <v>9</v>
+      </c>
+      <c r="C12" s="30">
+        <v>43099</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="30">
+        <v>43103</v>
+      </c>
+      <c r="G12" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="34"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>9</v>
-      </c>
-      <c r="C12" s="8">
-        <v>43099</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="35"/>
-      <c r="I12" s="10"/>
+      <c r="H12" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B13" s="29">
@@ -1656,10 +1675,10 @@
         <v>43099</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I13" s="34"/>
     </row>
@@ -1680,10 +1699,10 @@
         <v>43099</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I14" s="34"/>
     </row>
@@ -1695,7 +1714,7 @@
         <v>43099</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>40</v>
@@ -1704,10 +1723,10 @@
         <v>43100</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I15" s="34"/>
     </row>
@@ -1719,17 +1738,17 @@
         <v>43099</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="35" t="s">
         <v>77</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>78</v>
       </c>
       <c r="I16" s="10"/>
     </row>
@@ -1741,7 +1760,7 @@
         <v>43099</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>40</v>
@@ -1750,10 +1769,10 @@
         <v>43102</v>
       </c>
       <c r="G17" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="32" t="s">
         <v>74</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>75</v>
       </c>
       <c r="I17" s="34"/>
     </row>
@@ -1765,7 +1784,7 @@
         <v>43099</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>40</v>
@@ -1774,10 +1793,10 @@
         <v>43102</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I18" s="34"/>
     </row>
@@ -1789,7 +1808,7 @@
         <v>43100</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="31" t="s">
         <v>40</v>
@@ -1798,34 +1817,52 @@
         <v>43102</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I19" s="34"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
+      <c r="B20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C20" s="30">
+        <v>43100</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="30">
+        <v>43106</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" s="34"/>
+    </row>
+    <row r="21" spans="2:9" ht="66" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <v>18</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="8">
+        <v>43105</v>
+      </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="F21" s="8"/>
-      <c r="G21" s="25"/>
+      <c r="G21" s="25" t="s">
+        <v>99</v>
+      </c>
       <c r="H21" s="35"/>
       <c r="I21" s="10"/>
     </row>
@@ -1965,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2119,7 +2156,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>51</v>
@@ -2134,10 +2171,10 @@
         <v>43102</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="19" t="s">
         <v>23</v>
@@ -2149,10 +2186,10 @@
         <v>23</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="66" x14ac:dyDescent="0.3">
@@ -2164,22 +2201,22 @@
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>23</v>
       </c>
       <c r="G9" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="I9" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="J9" s="24" t="s">
         <v>85</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -2191,7 +2228,7 @@
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>23</v>
@@ -2200,13 +2237,13 @@
         <v>23</v>
       </c>
       <c r="H10" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>90</v>
-      </c>
       <c r="J10" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -2230,10 +2267,10 @@
         <v>35</v>
       </c>
       <c r="I11" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="41" t="s">
         <v>94</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SCH - MCU USART R/Tx Pin-swap  USART R/Tx pin 할당 miss
</commit_message>
<xml_diff>
--- a/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
+++ b/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -494,6 +494,40 @@
  - RX interrupt 인식을 못함
  - USART1_RX date의 Low level이 2.17V 까지밖에 안떨어짐(정상 0V)
  - MAX3232의 ChargePump의 파형이 점검치구 board와 틀림</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU의 Pin할당 miss
+ - PA9 : USART1_RX -&gt; USART1_TX
+ - PA10 : USART1_TX -&gt; USART1_RX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>U1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN-42(PA9) - USART1_RX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN-42(PA9) - USART1_TX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN-43(PA10) - USART1_RX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN-43(PA10) - USART1_TX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USART1 R/Tx Swap : Off-page 할당 miss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB 수정</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1388,8 +1422,8 @@
   <dimension ref="B1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1855,7 +1889,9 @@
       <c r="C21" s="8">
         <v>43105</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E21" s="3" t="s">
         <v>66</v>
       </c>
@@ -1863,7 +1899,9 @@
       <c r="G21" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="H21" s="35"/>
+      <c r="H21" s="35" t="s">
+        <v>100</v>
+      </c>
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -2003,7 +2041,7 @@
   <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2216,7 +2254,7 @@
         <v>84</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -2277,27 +2315,55 @@
       <c r="B12" s="54">
         <v>9</v>
       </c>
-      <c r="C12" s="55"/>
+      <c r="C12" s="55">
+        <v>43107</v>
+      </c>
       <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="57"/>
+      <c r="E12" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="J12" s="57" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="21">
         <v>10</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8">
+        <v>43107</v>
+      </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="24"/>
+      <c r="E13" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="21">

</xml_diff>

<commit_message>
SCH - RS-232 관련 NC part 추가
</commit_message>
<xml_diff>
--- a/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
+++ b/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Issue list" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="114">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -528,6 +528,32 @@
   </si>
   <si>
     <t>PCB 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C26</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAP NC 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX3232 T_OUT pin에 -5V Pull-up이 필요한 경우
+C8를  NC처리하고 C26에 0.1uF 실장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R37, R38</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Noise filtering or R/Tx pin swap용 저항</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_Main Board_SCH_V2.0_20180107.sch
+Plasma_Gen_Main Board_PCB_V2.0_20180107.pcb</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -933,7 +959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1114,6 +1140,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1175,7 +1204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1210,7 +1239,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1421,7 +1450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
@@ -2040,8 +2069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2311,14 +2340,16 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="33" x14ac:dyDescent="0.3">
       <c r="B12" s="54">
         <v>9</v>
       </c>
       <c r="C12" s="55">
         <v>43107</v>
       </c>
-      <c r="D12" s="56"/>
+      <c r="D12" s="61" t="s">
+        <v>113</v>
+      </c>
       <c r="E12" s="56" t="s">
         <v>101</v>
       </c>
@@ -2365,31 +2396,59 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="33" x14ac:dyDescent="0.3">
       <c r="B14" s="21">
         <v>11</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="8">
+        <v>43107</v>
+      </c>
       <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="24"/>
+      <c r="E14" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="21">
         <v>12</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="8">
+        <v>43107</v>
+      </c>
       <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="24"/>
+      <c r="E15" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="21">

</xml_diff>

<commit_message>
SCH - External only용 Dummy Res 추가
</commit_message>
<xml_diff>
--- a/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
+++ b/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="125">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -590,6 +590,15 @@
   </si>
   <si>
     <t>External Power용 Jumper Res</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery Type 결정에 따라 CON pin-map 및 부품 변경</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_Main Board_SCH_V2.0_20180114.sch
+Plasma_Gen_Main Board_PCB_V2.0_20180114.pcb</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1240,7 +1249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1275,7 +1284,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2019,11 +2028,19 @@
       <c r="B24" s="2">
         <v>21</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="C24" s="8">
+        <v>43115</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="25"/>
+      <c r="G24" s="25" t="s">
+        <v>123</v>
+      </c>
       <c r="H24" s="35"/>
       <c r="I24" s="10"/>
     </row>
@@ -2128,7 +2145,7 @@
   <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D23" sqref="D22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2508,14 +2525,16 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="33" x14ac:dyDescent="0.3">
       <c r="B16" s="21">
         <v>13</v>
       </c>
       <c r="C16" s="8">
         <v>43114</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="E16" s="22" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
SCH - HW_ID, Screw hole에 GND 추가
</commit_message>
<xml_diff>
--- a/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
+++ b/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
@@ -10,12 +10,13 @@
     <sheet name="Issue list" sheetId="1" r:id="rId1"/>
     <sheet name="ECO list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="141">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -581,10 +582,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>R39</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>NC</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -599,6 +596,80 @@
   <si>
     <t>Plasma_Gen_Main Board_SCH_V2.0_20180114.sch
 Plasma_Gen_Main Board_PCB_V2.0_20180114.pcb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW_ID0,1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW version
+ R40 :  NC, R41 : NC --&gt; 00 : portable version
+ R40 : 10K, R41 : NC --&gt; 01 : External Only version</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1, P2, P3, P4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drill Hole</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND와 연결</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Portable version에서 GND lead 선 연결용 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copper Keepout 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_Main Board_SCH_V2.0_20180120.sch
+Plasma_Gen_Main Board_PCB_V2.0_20180120.pcb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP시 Battery 없는 상태에서도 Booting 및 DL 가능하도록 지원
+ 1. Test Pin 추가
+ 2. 하나의 CON로 DL 가능하도록 지원 여부 검토(External Power Pin 할당)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R40,R41</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_ID에 연결</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>고전원 input시 Voltage divide 가능하도록 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW_ID0 : PA1, HW_ID1 : PA2 Pin 할당
+ R40,R41 Pull-up 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R39</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R39 추가</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1004,7 +1075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1188,6 +1259,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1496,8 +1588,8 @@
   <dimension ref="B1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1982,47 +2074,57 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
+    <row r="22" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="30">
         <v>43114</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="25" t="s">
+      <c r="E22" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="30">
+        <v>43120</v>
+      </c>
+      <c r="G22" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="H22" s="35"/>
-      <c r="I22" s="10" t="s">
+      <c r="H22" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" s="34" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="2">
+      <c r="B23" s="29">
         <v>20</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="30">
         <v>43114</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="25" t="s">
+      <c r="E23" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="30">
+        <v>43114</v>
+      </c>
+      <c r="G23" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="H23" s="35"/>
-      <c r="I23" s="10"/>
+      <c r="H23" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
@@ -2039,20 +2141,28 @@
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H24" s="35"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
         <v>22</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="C25" s="8">
+        <v>43120</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="F25" s="8"/>
-      <c r="G25" s="25"/>
+      <c r="G25" s="25" t="s">
+        <v>133</v>
+      </c>
       <c r="H25" s="35"/>
       <c r="I25" s="10"/>
     </row>
@@ -2144,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D22:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2498,113 +2608,171 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="21">
+    <row r="15" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="49">
         <v>12</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="50">
         <v>43107</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22" t="s">
+      <c r="D15" s="51"/>
+      <c r="E15" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="J15" s="53" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B16" s="21">
+    <row r="16" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="63">
         <v>13</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="64">
         <v>43114</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="I16" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="68" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="54">
+        <v>14</v>
+      </c>
+      <c r="C17" s="55">
+        <v>43120</v>
+      </c>
+      <c r="D17" s="61" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F16" s="23" t="s">
+      <c r="G17" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="J16" s="24" t="s">
+      <c r="H17" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="J17" s="57" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="21">
-        <v>14</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="24"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="21">
         <v>15</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8">
+        <v>43120</v>
+      </c>
       <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="24"/>
+      <c r="E18" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="21">
         <v>16</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="8">
+        <v>43120</v>
+      </c>
       <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="24"/>
+      <c r="E19" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="21">
         <v>17</v>
       </c>
-      <c r="C20" s="8"/>
+      <c r="C20" s="8">
+        <v>43120</v>
+      </c>
       <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="24"/>
+      <c r="E20" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="21">

</xml_diff>

<commit_message>
SCH - Gas input detect을 위한 수정  - CON 추가  - GAS_IN GPIO pin 추가  - Pull-up 저항 추가
</commit_message>
<xml_diff>
--- a/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
+++ b/1_Schematic/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
@@ -10,13 +10,12 @@
     <sheet name="Issue list" sheetId="1" r:id="rId1"/>
     <sheet name="ECO list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511" calcMode="manual" calcCompleted="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="149">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -406,10 +405,6 @@
   </si>
   <si>
     <t>R35, R36</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>10KΩ</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -670,6 +665,47 @@
   </si>
   <si>
     <t>R39 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas 주입 인식을 위한 신호 추가 - GPIO 1ea, GND 1ea, CON 2pin 1ea
+ - GPIO 신호 type : 
+       Gas Off : Open
+       Gas On : GND</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>J7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS_IN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS input detect을 위한 GPIO 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R42</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10KΩ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS input detect을 위한 Pull-up Res 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>12512WS-02B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>12512WS-02B CON 추가
+GAS_IN Pin 추가 : PC0
+Pull-up Res 10K 추가</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1589,7 +1625,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1658,7 +1694,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I4" s="48"/>
     </row>
@@ -1682,10 +1718,10 @@
         <v>11</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
@@ -1854,7 +1890,7 @@
         <v>57</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I12" s="34"/>
     </row>
@@ -2041,10 +2077,10 @@
         <v>43106</v>
       </c>
       <c r="G20" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="32" t="s">
         <v>97</v>
-      </c>
-      <c r="H20" s="32" t="s">
-        <v>98</v>
       </c>
       <c r="I20" s="34"/>
     </row>
@@ -2065,13 +2101,13 @@
         <v>43107</v>
       </c>
       <c r="G21" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="H21" s="32" t="s">
-        <v>100</v>
-      </c>
       <c r="I21" s="34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="33" x14ac:dyDescent="0.3">
@@ -2082,7 +2118,7 @@
         <v>43114</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" s="31" t="s">
         <v>40</v>
@@ -2091,13 +2127,13 @@
         <v>43120</v>
       </c>
       <c r="G22" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I22" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
@@ -2108,7 +2144,7 @@
         <v>43114</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E23" s="31" t="s">
         <v>40</v>
@@ -2117,13 +2153,13 @@
         <v>43114</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I23" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
@@ -2134,14 +2170,14 @@
         <v>43115</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H24" s="35"/>
       <c r="I24" s="10"/>
@@ -2154,29 +2190,43 @@
         <v>43120</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H25" s="35"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
+    <row r="26" spans="2:9" ht="66" x14ac:dyDescent="0.3">
+      <c r="B26" s="29">
         <v>23</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="10"/>
+      <c r="C26" s="30">
+        <v>43121</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="30">
+        <v>43121</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
@@ -2255,7 +2305,7 @@
   <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2408,7 +2458,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>51</v>
@@ -2423,7 +2473,7 @@
         <v>43102</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>79</v>
@@ -2468,7 +2518,7 @@
         <v>84</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -2489,10 +2539,10 @@
         <v>23</v>
       </c>
       <c r="H10" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" s="22" t="s">
         <v>88</v>
-      </c>
-      <c r="I10" s="22" t="s">
-        <v>89</v>
       </c>
       <c r="J10" s="24" t="s">
         <v>85</v>
@@ -2519,10 +2569,10 @@
         <v>35</v>
       </c>
       <c r="I11" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="41" t="s">
         <v>93</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="33" x14ac:dyDescent="0.3">
@@ -2533,25 +2583,25 @@
         <v>43107</v>
       </c>
       <c r="D12" s="61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="H12" s="56" t="s">
-        <v>103</v>
-      </c>
       <c r="I12" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="J12" s="57" t="s">
         <v>106</v>
-      </c>
-      <c r="J12" s="57" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
@@ -2563,22 +2613,22 @@
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H13" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" s="22" t="s">
+      <c r="J13" s="24" t="s">
         <v>106</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="33" x14ac:dyDescent="0.3">
@@ -2590,7 +2640,7 @@
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>23</v>
@@ -2599,10 +2649,10 @@
         <v>23</v>
       </c>
       <c r="H14" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14" s="25" t="s">
         <v>109</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>110</v>
       </c>
       <c r="J14" s="24" t="s">
         <v>85</v>
@@ -2617,7 +2667,7 @@
       </c>
       <c r="D15" s="51"/>
       <c r="E15" s="51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F15" s="52" t="s">
         <v>23</v>
@@ -2626,10 +2676,10 @@
         <v>23</v>
       </c>
       <c r="H15" s="51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I15" s="51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J15" s="53" t="s">
         <v>85</v>
@@ -2643,10 +2693,10 @@
         <v>43114</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E16" s="66" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F16" s="67" t="s">
         <v>23</v>
@@ -2655,10 +2705,10 @@
         <v>23</v>
       </c>
       <c r="H16" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" s="66" t="s">
         <v>120</v>
-      </c>
-      <c r="I16" s="66" t="s">
-        <v>121</v>
       </c>
       <c r="J16" s="68" t="s">
         <v>85</v>
@@ -2672,22 +2722,22 @@
         <v>43120</v>
       </c>
       <c r="D17" s="61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E17" s="56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" s="62" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" s="61" t="s">
         <v>125</v>
-      </c>
-      <c r="I17" s="61" t="s">
-        <v>126</v>
       </c>
       <c r="J17" s="57" t="s">
         <v>85</v>
@@ -2702,19 +2752,19 @@
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="I18" s="22" t="s">
         <v>129</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>130</v>
       </c>
       <c r="J18" s="24" t="s">
         <v>85</v>
@@ -2729,7 +2779,7 @@
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>23</v>
@@ -2738,10 +2788,10 @@
         <v>23</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J19" s="24" t="s">
         <v>85</v>
@@ -2756,7 +2806,7 @@
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>23</v>
@@ -2765,10 +2815,10 @@
         <v>23</v>
       </c>
       <c r="H20" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="I20" s="22" t="s">
         <v>136</v>
-      </c>
-      <c r="I20" s="22" t="s">
-        <v>137</v>
       </c>
       <c r="J20" s="24" t="s">
         <v>85</v>
@@ -2778,26 +2828,50 @@
       <c r="B21" s="21">
         <v>18</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="8">
+        <v>43120</v>
+      </c>
       <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
+      <c r="E21" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>143</v>
+      </c>
       <c r="J21" s="24"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="21">
         <v>19</v>
       </c>
-      <c r="C22" s="8"/>
+      <c r="C22" s="8">
+        <v>43120</v>
+      </c>
       <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
+      <c r="E22" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>146</v>
+      </c>
       <c r="J22" s="24"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">

</xml_diff>